<commit_message>
chore: personalize defaults to Pranav and exclude env changes
Update README, config, UI templates, and UI settings to use Pranav’s details. Exclude `env.example` changes (stashed locally) to avoid pushing secrets.
</commit_message>
<xml_diff>
--- a/data/sent.xlsx
+++ b/data/sent.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:D49"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -976,9 +976,121 @@
         <v/>
       </c>
     </row>
+    <row r="42">
+      <c r="A42" t="str">
+        <v>harshal.patil@thinkitive.com</v>
+      </c>
+      <c r="B42" t="str">
+        <v>Harshal Patil</v>
+      </c>
+      <c r="C42" t="str">
+        <v>Application for MERN Stack Developer Role — Immediate Joiner | 3 Yrs Experience</v>
+      </c>
+      <c r="D42" t="str">
+        <v>Resume not found at /Users/pranavwaykar/var/www/My Projects/JobPilot/assets/Pranav_Waykar.pdf. Put your PDF there or set RESUME_PATH in .env</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="str">
+        <v>harshal.patil@thinkitive.com</v>
+      </c>
+      <c r="B43" t="str">
+        <v>Harshal Patil</v>
+      </c>
+      <c r="C43" t="str">
+        <v>Application for MERN Stack Developer Role — Immediate Joiner | 3 Yrs Experience</v>
+      </c>
+      <c r="D43" t="str">
+        <v>Resume not found at /Users/pranavwaykar/var/www/My Projects/JobPilot/assets/Pranav_Waykar.pdf. Put your PDF there or set RESUME_PATH in .env</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="str">
+        <v>harshal.patil@thinkitive.com</v>
+      </c>
+      <c r="B44" t="str">
+        <v>Harshal Patil</v>
+      </c>
+      <c r="C44" t="str">
+        <v>Application for MERN Stack Developer Role — Immediate Joiner | 3 Yrs Experience</v>
+      </c>
+      <c r="D44" t="str">
+        <v>Resume not found at /Users/pranavwaykar/var/www/My Projects/JobPilot/assets/Pranav_Waykar.pdf. Put your PDF there or set RESUME_PATH in .env</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="str">
+        <v>ganeshvarahade@thinkitive.com</v>
+      </c>
+      <c r="B45" t="str">
+        <v>Ganesh Varahade</v>
+      </c>
+      <c r="C45" t="str">
+        <v>Application for MERN Stack Developer Role — Immediate Joiner | 3 Yrs Experience</v>
+      </c>
+      <c r="D45" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="str">
+        <v>dhananjay.kolte@thinkitive.com</v>
+      </c>
+      <c r="B46" t="str">
+        <v>Dhananjay Kolte</v>
+      </c>
+      <c r="C46" t="str">
+        <v>Application for MERN Stack Developer Role — Immediate Joiner | 3 Yrs Experience</v>
+      </c>
+      <c r="D46" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="str">
+        <v>harshal.patil@thinkitive.com</v>
+      </c>
+      <c r="B47" t="str">
+        <v>Harshal Patil</v>
+      </c>
+      <c r="C47" t="str">
+        <v>Application for MERN Stack Developer Role — Immediate Joiner | 3 Yrs Experience</v>
+      </c>
+      <c r="D47" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="str">
+        <v>waykarpranav777@gmail.com</v>
+      </c>
+      <c r="B48" t="str">
+        <v/>
+      </c>
+      <c r="C48" t="str">
+        <v>Application for MERN Stack Developer Role — Immediate Joiner | 3 Yrs Experience</v>
+      </c>
+      <c r="D48" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="str">
+        <v>waykarpranav777@gmail.com</v>
+      </c>
+      <c r="B49" t="str">
+        <v/>
+      </c>
+      <c r="C49" t="str">
+        <v>Application for MERN Stack Developer Role — Immediate Joiner | 3 Yrs Experience</v>
+      </c>
+      <c r="D49" t="str">
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D41"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D49"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>